<commit_message>
adde AdderPlus and RCA to reports
</commit_message>
<xml_diff>
--- a/Project_1/Reports.xlsx
+++ b/Project_1/Reports.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1st Semester\VLSI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\academic_material\third_year\VLSI\repos\VLSI-Projects\Project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CECB94-16D0-46B6-BB8F-CC159414CF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0"/>
+    <workbookView xWindow="11712" yWindow="4560" windowWidth="8940" windowHeight="9588" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="26">
   <si>
     <t>Carry Save Adder</t>
   </si>
@@ -72,12 +73,42 @@
   </si>
   <si>
     <t>Carry Select Adder</t>
+  </si>
+  <si>
+    <t>Ripple Carry Adder</t>
+  </si>
+  <si>
+    <t>-----+-----------+-----</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     |Unit       |Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1    |Time       |ns   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2    |Capacitance|ff   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3    |Resistance |kohm </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4    |Power      |nW   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5    |Voltage    |V    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6    |Current    |mA   </t>
+  </si>
+  <si>
+    <t>Simple Adder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -142,13 +173,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -430,11 +461,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A14:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,376 +478,600 @@
     <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+    <row r="14" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>19500</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2582.9</v>
+      </c>
+      <c r="C17" s="1">
+        <v>16917.099999999999</v>
+      </c>
+      <c r="D17" s="1">
+        <v>8.3133579999999991</v>
+      </c>
+      <c r="E17" s="1">
+        <v>17.327546999999999</v>
+      </c>
+      <c r="F17" s="1">
+        <v>4.2053859999999998</v>
+      </c>
+      <c r="G17" s="1">
+        <v>29.846291999999998</v>
+      </c>
+      <c r="H17" s="1">
+        <v>161</v>
+      </c>
+      <c r="I17" s="1">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="A22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>19500</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2582.9</v>
+      </c>
+      <c r="C25" s="1">
+        <v>16917.099999999999</v>
+      </c>
+      <c r="D25" s="1">
+        <v>8.3133579999999991</v>
+      </c>
+      <c r="E25" s="1">
+        <v>17.327546999999999</v>
+      </c>
+      <c r="F25" s="1">
+        <v>4.2053859999999998</v>
+      </c>
+      <c r="G25" s="1">
+        <v>29.846291999999998</v>
+      </c>
+      <c r="H25" s="1">
+        <v>161</v>
+      </c>
+      <c r="I25" s="1">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+      <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I31" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
         <v>19500</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B32" s="1">
         <v>2582.1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C32" s="1">
         <v>16917.900000000001</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D32" s="1">
         <v>16.183603000000002</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E32" s="1">
         <v>31.498101999999999</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F32" s="1">
         <v>8.2003210000000006</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G32" s="1">
         <v>55.882022999999997</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H32" s="1">
         <v>314</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I32" s="1">
         <v>368</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
+    <row r="34" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A34" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
         <v>19500</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B37" s="1">
         <v>2841.6</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C37" s="1">
         <v>16658.400000000001</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D37" s="1">
         <v>6.8695329999999997</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E37" s="1">
         <v>20.417660000000001</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F37" s="1">
         <v>3.5430000000000001</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G37" s="1">
         <v>30.830193000000001</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H37" s="1">
         <v>120</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I37" s="1">
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
+    <row r="39" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A39" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A40" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3" t="s">
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F41" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
         <v>19500</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B42" s="1">
         <v>2339.6999999999998</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C42" s="1">
         <v>17160.3</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D42" s="1">
         <v>10.643272</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E42" s="1">
         <v>18.815377999999999</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F42" s="1">
         <v>5.5814250000000003</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G42" s="1">
         <v>35.040076999999997</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H42" s="1">
         <v>203</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I42" s="1">
         <v>247</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="21" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
+      <c r="N42" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N43" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A44" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="N44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3" t="s">
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="I45" s="4"/>
+      <c r="N45" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F46" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+      <c r="N46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
         <v>19500</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B47" s="1">
         <v>1813.2</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C47" s="1">
         <v>17686.8</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D47" s="1">
         <v>16.417072000000001</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E47" s="1">
         <v>24.459493999999999</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F47" s="1">
         <v>8.1156229999999994</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G47" s="1">
         <v>48.992190999999998</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H47" s="1">
         <v>294</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I47" s="1">
         <v>372</v>
       </c>
+      <c r="N47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N51" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A16:I16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A6:I6"/>
+  <mergeCells count="24">
+    <mergeCell ref="A22:I22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="A14:I14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="A34:I34"/>
+    <mergeCell ref="A44:I44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="A39:I39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="D40:G40"/>
+    <mergeCell ref="H40:I40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>